<commit_message>
3/11/2016 -- St. Louis Competition -- Day 2
</commit_message>
<xml_diff>
--- a/Auto Mode List.xlsx
+++ b/Auto Mode List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="72" windowWidth="20112" windowHeight="7992"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t xml:space="preserve">Cheval De Frise </t>
   </si>
@@ -38,9 +38,6 @@
     <t>MODE #</t>
   </si>
   <si>
-    <t>Low Bar</t>
-  </si>
-  <si>
     <t>Drawbridge - Not implemented</t>
   </si>
   <si>
@@ -54,6 +51,15 @@
   </si>
   <si>
     <t>Autonomous Modes</t>
+  </si>
+  <si>
+    <t>Low Bar (Close with /targetTrack)</t>
+  </si>
+  <si>
+    <t>Low Bar (Far with /targetTrack)</t>
+  </si>
+  <si>
+    <t>default</t>
   </si>
 </sst>
 </file>
@@ -453,21 +459,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B12"/>
+      <selection activeCell="B14" sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="6"/>
     </row>
@@ -484,7 +490,7 @@
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -516,7 +522,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -524,7 +530,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -532,7 +538,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -556,7 +562,23 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -574,7 +596,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Salty Post Spring Break Code Incomplete Started 2 ball.  Long shot
</commit_message>
<xml_diff>
--- a/Auto Mode List.xlsx
+++ b/Auto Mode List.xlsx
@@ -15,19 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
-  <si>
-    <t xml:space="preserve">Cheval De Frise </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moat </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ramparts </t>
-  </si>
-  <si>
-    <t>Rough Terrain</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Corner Shot</t>
   </si>
@@ -38,35 +26,32 @@
     <t>MODE #</t>
   </si>
   <si>
-    <t>Drawbridge - Not implemented</t>
-  </si>
-  <si>
-    <t>Rock Wall  - Not implemented</t>
-  </si>
-  <si>
-    <t>Sally Port  - Not implemented</t>
-  </si>
-  <si>
-    <t>Portcullis  - Not implemented</t>
-  </si>
-  <si>
     <t>Autonomous Modes</t>
   </si>
   <si>
-    <t>Low Bar (Close with /targetTrack)</t>
-  </si>
-  <si>
-    <t>Low Bar (Far with /targetTrack)</t>
-  </si>
-  <si>
     <t>default</t>
+  </si>
+  <si>
+    <t>Low Bar w gyro</t>
+  </si>
+  <si>
+    <t>Portcullis  w gyro</t>
+  </si>
+  <si>
+    <t>Cheval De Frise w gyro</t>
+  </si>
+  <si>
+    <t>Moat w gyro</t>
+  </si>
+  <si>
+    <t>Low Bar w gyro, 2 ball w spy bot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +91,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -139,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -153,6 +146,13 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="A1:B14"/>
+      <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,112 +473,72 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B1" s="6"/>
     </row>
     <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="7">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="7">
+        <v>100</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="8">
+        <v>101</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="7">
+        <v>102</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>103</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="8">
+        <v>200</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>7</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>8</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>9</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>21</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -586,7 +546,7 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated image to what is working for Cincy regional
</commit_message>
<xml_diff>
--- a/Auto Mode List.xlsx
+++ b/Auto Mode List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="72" windowWidth="20112" windowHeight="7992"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -15,19 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
-  <si>
-    <t xml:space="preserve">Cheval De Frise </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moat </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ramparts </t>
-  </si>
-  <si>
-    <t>Rough Terrain</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Corner Shot</t>
   </si>
@@ -38,35 +26,32 @@
     <t>MODE #</t>
   </si>
   <si>
-    <t>Drawbridge - Not implemented</t>
-  </si>
-  <si>
-    <t>Rock Wall  - Not implemented</t>
-  </si>
-  <si>
-    <t>Sally Port  - Not implemented</t>
-  </si>
-  <si>
-    <t>Portcullis  - Not implemented</t>
-  </si>
-  <si>
     <t>Autonomous Modes</t>
   </si>
   <si>
-    <t>Low Bar (Close with /targetTrack)</t>
-  </si>
-  <si>
-    <t>Low Bar (Far with /targetTrack)</t>
-  </si>
-  <si>
     <t>default</t>
+  </si>
+  <si>
+    <t>Low Bar One Ball (w Gyro)</t>
+  </si>
+  <si>
+    <t>Portcullis One Ball (w Gyro)</t>
+  </si>
+  <si>
+    <t>Cheval One Ball (w Gyro)</t>
+  </si>
+  <si>
+    <t>Rough Terrain One Ball (w Gyro)</t>
+  </si>
+  <si>
+    <t>Low Bar Two Ball  w Spybot (w Gyro)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +91,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -139,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -153,6 +146,13 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,126 +459,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="A1:B14"/>
+      <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>100</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>101</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>102</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>103</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>200</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>7</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>8</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>9</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>21</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -596,7 +556,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finally getting around to pushing the code from Queen City Regional, which we won! Everything is more or less working, but everybody wants some improvements made.
</commit_message>
<xml_diff>
--- a/Auto Mode List.xlsx
+++ b/Auto Mode List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="72" windowWidth="20112" windowHeight="7992"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -15,19 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
-  <si>
-    <t xml:space="preserve">Cheval De Frise </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moat </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ramparts </t>
-  </si>
-  <si>
-    <t>Rough Terrain</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Corner Shot</t>
   </si>
@@ -38,35 +26,32 @@
     <t>MODE #</t>
   </si>
   <si>
-    <t>Drawbridge - Not implemented</t>
-  </si>
-  <si>
-    <t>Rock Wall  - Not implemented</t>
-  </si>
-  <si>
-    <t>Sally Port  - Not implemented</t>
-  </si>
-  <si>
-    <t>Portcullis  - Not implemented</t>
-  </si>
-  <si>
     <t>Autonomous Modes</t>
   </si>
   <si>
-    <t>Low Bar (Close with /targetTrack)</t>
-  </si>
-  <si>
-    <t>Low Bar (Far with /targetTrack)</t>
-  </si>
-  <si>
     <t>default</t>
+  </si>
+  <si>
+    <t>Low Bar One Ball (w Gyro)</t>
+  </si>
+  <si>
+    <t>Portcullis One Ball (w Gyro)</t>
+  </si>
+  <si>
+    <t>Cheval One Ball (w Gyro)</t>
+  </si>
+  <si>
+    <t>Rough Terrain One Ball (w Gyro)</t>
+  </si>
+  <si>
+    <t>Low Bar Two Ball  w Spybot (w Gyro)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +91,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -139,7 +132,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -153,6 +146,13 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,126 +459,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="A1:B14"/>
+      <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B1" s="6"/>
     </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="7">
+        <v>8</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7">
+        <v>100</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7">
+        <v>101</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>102</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>103</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>200</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>4</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>5</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
-        <v>6</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
-        <v>7</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>8</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>9</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>21</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -596,7 +556,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "Updated image to what is working for Cincy regional"
This reverts commit 0271860ee37c11ac73770228752539d65fcaa3f3.
</commit_message>
<xml_diff>
--- a/Auto Mode List.xlsx
+++ b/Auto Mode List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="72" windowWidth="20112" windowHeight="7992"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+  <si>
+    <t xml:space="preserve">Cheval De Frise </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ramparts </t>
+  </si>
+  <si>
+    <t>Rough Terrain</t>
+  </si>
   <si>
     <t>Corner Shot</t>
   </si>
@@ -26,32 +38,35 @@
     <t>MODE #</t>
   </si>
   <si>
+    <t>Drawbridge - Not implemented</t>
+  </si>
+  <si>
+    <t>Rock Wall  - Not implemented</t>
+  </si>
+  <si>
+    <t>Sally Port  - Not implemented</t>
+  </si>
+  <si>
+    <t>Portcullis  - Not implemented</t>
+  </si>
+  <si>
     <t>Autonomous Modes</t>
   </si>
   <si>
+    <t>Low Bar (Close with /targetTrack)</t>
+  </si>
+  <si>
+    <t>Low Bar (Far with /targetTrack)</t>
+  </si>
+  <si>
     <t>default</t>
-  </si>
-  <si>
-    <t>Low Bar One Ball (w Gyro)</t>
-  </si>
-  <si>
-    <t>Portcullis One Ball (w Gyro)</t>
-  </si>
-  <si>
-    <t>Cheval One Ball (w Gyro)</t>
-  </si>
-  <si>
-    <t>Rough Terrain One Ball (w Gyro)</t>
-  </si>
-  <si>
-    <t>Low Bar Two Ball  w Spybot (w Gyro)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,14 +106,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFF00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -132,7 +139,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -146,13 +153,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,86 +459,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B9"/>
+      <selection activeCell="B14" sqref="A1:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="6"/>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="B6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>6</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>100</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>101</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>102</v>
-      </c>
-      <c r="B6" s="5" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
-        <v>103</v>
-      </c>
-      <c r="B7" s="5" t="s">
+      <c r="B10" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>200</v>
-      </c>
-      <c r="B8" s="9" t="s">
+      <c r="B11" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="B12" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>21</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -556,7 +596,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated smart dashboard with latest autos
</commit_message>
<xml_diff>
--- a/Auto Mode List.xlsx
+++ b/Auto Mode List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="240" yWindow="72" windowWidth="20112" windowHeight="7992"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Corner Shot</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Low Bar Two Ball  w Spybot (w Gyro)</t>
+  </si>
+  <si>
+    <t>Rock Wall One Ball (w Gyro)</t>
   </si>
 </sst>
 </file>
@@ -143,9 +146,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -153,6 +153,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,19 +468,19 @@
       <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.45" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6"/>
-    </row>
-    <row r="2" spans="1:2" s="1" customFormat="1" ht="14.45" x14ac:dyDescent="0.25">
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -485,56 +488,56 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+    <row r="3" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>100</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>101</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>102</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>103</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>100</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7">
-        <v>101</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>102</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
-        <v>103</v>
+    </row>
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>104</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
         <v>200</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -556,7 +559,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>